<commit_message>
comparison between emta and excel edded.
</commit_message>
<xml_diff>
--- a/src/main/resources/U5646616_2021_2021.xlsx
+++ b/src/main/resources/U5646616_2021_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indre\IdeaProjects\taxFormFiller\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657B8A99-552F-4D17-9C22-F0427B2FC850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2183609-E688-4384-AB0E-80AF64AB5E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="U5646616_2021_2021" sheetId="1" r:id="rId1"/>
@@ -26131,11 +26131,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724CC0B6-5A09-458C-B4E3-582AB8DBA603}">
-  <dimension ref="A1:P111"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32551,6 +32551,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G113" s="7">
+        <f ca="1">I111-G111</f>
+        <v>-303.67999999998574</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G114" s="7">
+        <f ca="1">-H111</f>
+        <v>-108.62999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G115" s="7">
+        <f ca="1">SUM(G113:G114)</f>
+        <v>-412.30999999998573</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G116" s="7">
+        <v>-345.63</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G117" s="7">
+        <f ca="1">G115/G116</f>
+        <v>1.1929230680206746</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32561,7 +32590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A617EC5-69E2-4458-95CC-9F54FE0EA36C}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>